<commit_message>
Ajout de Mesures de l'optimisation 1 + Correction du sens de l'optimisation 1.
</commit_message>
<xml_diff>
--- a/Mesures/1 - Mesures.xlsx
+++ b/Mesures/1 - Mesures.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Documents\Temporaire\FISE2\OPTION1\HPP\Projet_Coronavirus\HPP_Coronavirus_Project\Mesures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCCE809-6BD8-4E7A-B900-68FD8BCA0EC7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2024687-C101-4F66-8BC6-42CD70D2E01C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" activeTab="1" xr2:uid="{3ECF27EF-CF39-47C0-885E-284BADAE2FC9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" activeTab="2" xr2:uid="{3ECF27EF-CF39-47C0-885E-284BADAE2FC9}"/>
   </bookViews>
   <sheets>
-    <sheet name="1" sheetId="1" r:id="rId1"/>
-    <sheet name="2" sheetId="2" r:id="rId2"/>
+    <sheet name="Base" sheetId="3" r:id="rId1"/>
+    <sheet name="Optimisation Mono" sheetId="2" r:id="rId2"/>
+    <sheet name="Graphiques" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>Itérations</t>
   </si>
@@ -73,23 +74,27 @@
     <t>ms =</t>
   </si>
   <si>
-    <t>-</t>
+    <t>Monothread - Affichage Syso - Correction : chaines unifiées ssi personne contaminatrice &lt; 14j</t>
   </si>
   <si>
-    <t>Monothread - Affichage Syso - chaines totalement unifiées</t>
-  </si>
-  <si>
-    <t>Monothread - Affichage Syso - Correction : chaines unifiées ssi personne contaminatrice &lt; 14j</t>
+    <t>Monothread - Affichage Syso - Correction : chaines unifiées</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -103,7 +108,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -208,45 +213,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -330,11 +296,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -345,16 +324,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,9 +405,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>mesures avec affichage Syso</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -450,214 +427,116 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="fr-FR"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="3"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'1'!$A$4:$A$23</c:f>
+              <c:f>Base!$A$4:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5000</c:v>
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10000</c:v>
+                  <c:v>30000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20000</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30000</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40000</c:v>
+                  <c:v>60000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50000</c:v>
+                  <c:v>70000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>60000</c:v>
+                  <c:v>80000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>70000</c:v>
+                  <c:v>90000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>80000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>90000</c:v>
+                  <c:v>120000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>100000</c:v>
+                  <c:v>140000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>120000</c:v>
+                  <c:v>160000</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>140000</c:v>
+                  <c:v>180000</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>200000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>250000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>300000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>400000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>510000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1'!$F$4:$F$23</c:f>
+              <c:f>Base!$F$4:$F$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>940</c:v>
+                  <c:v>18240</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5420</c:v>
+                  <c:v>72940</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18600</c:v>
+                  <c:v>191340</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>69960</c:v>
+                  <c:v>341210</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>165760</c:v>
+                  <c:v>561320</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>356630</c:v>
+                  <c:v>830530</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>568670</c:v>
+                  <c:v>1118400</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>859920</c:v>
+                  <c:v>1441280</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1177460</c:v>
+                  <c:v>1821780</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1568300</c:v>
+                  <c:v>2252660</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1962280</c:v>
+                  <c:v>3205080</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2316380</c:v>
+                  <c:v>4326370</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3212320</c:v>
+                  <c:v>5770790</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4271810</c:v>
+                  <c:v>7102430</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8087510</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>12547900</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18021800</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>31590800</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>61326870</c:v>
+                  <c:v>8451140</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -665,7 +544,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4983-40F7-9C88-DFD6A233F021}"/>
+              <c16:uniqueId val="{00000000-2D52-4692-9601-B7B77F10DFD9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -677,11 +556,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="430735824"/>
-        <c:axId val="300048192"/>
+        <c:axId val="737746511"/>
+        <c:axId val="740227007"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="430735824"/>
+        <c:axId val="737746511"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -738,12 +617,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300048192"/>
+        <c:crossAx val="740227007"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="300048192"/>
+        <c:axId val="740227007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -800,7 +679,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="430735824"/>
+        <c:crossAx val="737746511"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -871,31 +750,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>mesures </a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -934,9 +788,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>mesures avec affichage Syso</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -969,25 +820,17 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:trendlineType val="poly"/>
             <c:order val="2"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.29444772528433943"/>
+                  <c:y val="5.0509259259259261E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1018,98 +861,116 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="3"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'2'!$A$4:$A$23</c:f>
+              <c:f>'Optimisation Mono'!$A$4:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5000</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10000</c:v>
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20000</c:v>
+                  <c:v>30000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30000</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40000</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50000</c:v>
+                  <c:v>60000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60000</c:v>
+                  <c:v>70000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>70000</c:v>
+                  <c:v>80000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80000</c:v>
+                  <c:v>90000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>90000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>100000</c:v>
+                  <c:v>120000</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>120000</c:v>
+                  <c:v>140000</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>140000</c:v>
+                  <c:v>160000</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>200000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>250000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>300000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>400000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>510000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>600000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'2'!$F$4:$F$23</c:f>
+              <c:f>'Optimisation Mono'!$F$4:$F$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16450</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60970</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>137970</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>245600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>401710</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>588840</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>842140</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1129100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1509000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1913900</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2965570</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4262530</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5437400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6718250</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8099510</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1117,7 +978,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-05D2-49F1-8C0B-D13A604C369D}"/>
+              <c16:uniqueId val="{00000000-A60B-4641-8FB9-812B9EC19FEA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1129,11 +990,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="430735824"/>
-        <c:axId val="300048192"/>
+        <c:axId val="596733903"/>
+        <c:axId val="740232831"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="430735824"/>
+        <c:axId val="596733903"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1190,12 +1051,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="300048192"/>
+        <c:crossAx val="740232831"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="300048192"/>
+        <c:axId val="740232831"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1252,7 +1113,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="430735824"/>
+        <c:crossAx val="596733903"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1264,6 +1125,572 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Programme fonctionnel initial</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Base!$A$4:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Base!$F$4:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18240</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72940</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>191340</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>341210</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>561320</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>830530</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1118400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1441280</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1821780</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2252660</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3205080</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4326370</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5770790</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7102430</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8451140</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8458-4175-AE98-42E7A1A99229}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Optimisation 1 - Ajout d'un indice indiquant la première personne dont score &gt; 0</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Optimisation Mono'!$A$4:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Optimisation Mono'!$F$4:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16450</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60970</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>137970</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>245600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>401710</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>588840</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>842140</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1129100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1509000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1913900</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2965570</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4262530</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5437400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6718250</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8099510</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8458-4175-AE98-42E7A1A99229}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="737794719"/>
+        <c:axId val="641735583"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="737794719"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="641735583"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="641735583"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="737794719"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1388,6 +1815,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1905,6 +2372,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2425,22 +3408,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>41275</xdr:rowOff>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>22225</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Graphique 1">
+        <xdr:cNvPr id="3" name="Graphique 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2892B2C5-6547-4BED-B389-39D269BC72D9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C4D720D-02D6-4197-9A73-95D57DBEFB97}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2465,29 +3448,68 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>41275</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>22225</xdr:rowOff>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graphique 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72C0246E-2784-41EC-9250-34B1C543613E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{514E817B-D163-4549-B72E-A9D21D6E4FA8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EC0A24B-A5C4-482A-AA74-848E1B8D88EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2800,11 +3822,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DA1CEC6-D122-429A-AC4A-C550C16EF90B}">
-  <dimension ref="A1:M49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B65D92B8-4D2A-433F-A1DF-3854FD50ED45}">
+  <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2829,22 +3851,22 @@
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="9" t="s">
         <v>5</v>
       </c>
       <c r="G3">
@@ -2861,27 +3883,27 @@
       </c>
       <c r="M3">
         <f>ROUNDDOWN(J4/86400000,0)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="7">
-        <v>0</v>
-      </c>
-      <c r="B4" s="8">
-        <v>0</v>
-      </c>
-      <c r="C4" s="8">
-        <v>0</v>
-      </c>
-      <c r="D4" s="8">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8">
+      <c r="A4" s="11">
+        <v>0</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12">
         <f>0*$G$3</f>
         <v>0</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="13">
         <f>E4+D4*1000+C4*60000+B4*3600000</f>
         <v>0</v>
       </c>
@@ -2889,20 +3911,20 @@
         <v>11</v>
       </c>
       <c r="J4">
-        <f>0.0003 * J3 * J3 - 16.787 * J3 +657994</f>
-        <v>283870994</v>
+        <f>0.0002 * J3 * J3 - 0.1033 * J3 - 22875</f>
+        <v>199873825</v>
       </c>
       <c r="L4" t="s">
         <v>8</v>
       </c>
       <c r="M4">
         <f>ROUNDDOWN((J4/86400000 - ROUNDDOWN(J4/86400000,0) )* 24,0)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -2911,325 +3933,325 @@
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1">
+        <f>0.24*$G$3</f>
+        <v>240</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" ref="F5:F19" si="0">E5+D5*1000+C5*60000+B5*3600000</f>
+        <v>18240</v>
+      </c>
+      <c r="L5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5">
+        <f>ROUNDDOWN(((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60,0)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>20000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>12</v>
+      </c>
+      <c r="E6" s="15">
         <f>0.94*$G$3</f>
         <v>940</v>
       </c>
-      <c r="F5" s="3">
-        <f t="shared" ref="F5:F23" si="0">E5+D5*1000+C5*60000+B5*3600000</f>
-        <v>940</v>
-      </c>
-      <c r="L5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M5">
-        <f>ROUNDDOWN(((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60,0)</f>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
-        <v>5000</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>5</v>
-      </c>
-      <c r="E6" s="1">
-        <f>0.42*$G$3</f>
-        <v>420</v>
-      </c>
       <c r="F6" s="3">
         <f t="shared" si="0"/>
-        <v>5420</v>
+        <v>72940</v>
       </c>
       <c r="L6" t="s">
         <v>10</v>
       </c>
       <c r="M6">
         <f>ROUNDDOWN((((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60 - M5) * 60,0)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
-        <v>10000</v>
+        <v>30000</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
       </c>
       <c r="C7" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E7" s="1">
-        <f>0.6*$G$3</f>
-        <v>600</v>
+        <f>0.34*$G$3</f>
+        <v>340</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" si="0"/>
-        <v>18600</v>
+        <v>191340</v>
       </c>
       <c r="L7" t="s">
         <v>12</v>
       </c>
       <c r="M7">
         <f>((((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60 - M5) * 60 - M6) * 1000</f>
-        <v>994.00000000599675</v>
+        <v>824.99999999083684</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
       </c>
       <c r="C8" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="E8" s="1">
-        <f>0.96*$G$3</f>
-        <v>960</v>
+        <f>0.21*$G$3</f>
+        <v>210</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
-        <v>69960</v>
+        <v>341210</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
       </c>
       <c r="C9" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D9" s="1">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="E9" s="1">
-        <f>0.76*$G$3</f>
-        <v>760</v>
+        <f>0.32*$G$3</f>
+        <v>320</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="0"/>
-        <v>165760</v>
+        <v>561320</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
-        <v>40000</v>
+        <v>60000</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
       </c>
       <c r="C10" s="1">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D10" s="1">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E10" s="1">
-        <f>0.63*$G$3</f>
-        <v>630</v>
+        <f>0.53*$G$3</f>
+        <v>530</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
-        <v>356630</v>
+        <v>830530</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
-        <v>50000</v>
+        <v>70000</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
       </c>
       <c r="C11" s="1">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E11" s="1">
-        <f>0.67*$G$3</f>
-        <v>670</v>
+        <f>0.4*$G$3</f>
+        <v>400</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" si="0"/>
-        <v>568670</v>
+        <v>1118400</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
-        <v>60000</v>
+        <v>80000</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
       </c>
       <c r="C12" s="1">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E12" s="1">
-        <f>0.92*$G$3</f>
-        <v>920</v>
+        <f>0.28*$G$3</f>
+        <v>280</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
-        <v>859920</v>
+        <v>1441280</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
-        <v>70000</v>
+        <v>90000</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
       </c>
       <c r="C13" s="1">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E13" s="1">
-        <f>0.46*$G$3</f>
-        <v>460</v>
+        <f>0.78*$G$3</f>
+        <v>780</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="0"/>
-        <v>1177460</v>
+        <v>1821780</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
-        <v>80000</v>
+        <v>100000</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
       </c>
       <c r="C14" s="1">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D14" s="1">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E14" s="1">
-        <f>0.3*$G$3</f>
-        <v>300</v>
+        <f>0.66*$G$3</f>
+        <v>660</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="0"/>
-        <v>1568300</v>
+        <v>2252660</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
-        <v>90000</v>
+        <v>120000</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
       </c>
       <c r="C15" s="1">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="E15" s="1">
-        <f>0.28*$G$3</f>
-        <v>280</v>
+        <f>0.08*$G$3</f>
+        <v>80</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="0"/>
-        <v>1962280</v>
+        <v>3205080</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
-        <v>100000</v>
+        <v>140000</v>
       </c>
       <c r="B16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="D16" s="1">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="E16" s="1">
-        <f>0.38*$G$3</f>
-        <v>380</v>
+        <f>0.37*$G$3</f>
+        <v>370</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="0"/>
-        <v>2316380</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+        <v>4326370</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
-        <v>120000</v>
+        <v>160000</v>
       </c>
       <c r="B17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D17" s="1">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E17" s="1">
-        <f>0.32*$G$3</f>
-        <v>320</v>
+        <f>0.79*$G$3</f>
+        <v>790</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="0"/>
-        <v>3212320</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+        <v>5770790</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
-        <v>140000</v>
+        <v>180000</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
       </c>
       <c r="C18" s="1">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="D18" s="1">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E18" s="1">
-        <f>0.81*$G$3</f>
-        <v>810</v>
+        <f>0.43*$G$3</f>
+        <v>430</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="0"/>
-        <v>4271810</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+        <v>7102430</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>200000</v>
       </c>
@@ -3237,369 +4259,386 @@
         <v>2</v>
       </c>
       <c r="C19" s="1">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D19" s="1">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E19" s="1">
-        <f>0.51*$G$3</f>
-        <v>510</v>
+        <f>0.14*$G$3</f>
+        <v>140</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="0"/>
-        <v>8087510</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+        <v>8451140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>250000</v>
       </c>
       <c r="B20" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C20" s="1">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="D20" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E20" s="1">
-        <f>0.9*$G$3</f>
-        <v>900</v>
+        <f t="shared" ref="E8:E28" si="1">0*$G$3</f>
+        <v>0</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" si="0"/>
-        <v>12547900</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>300000</v>
       </c>
       <c r="B21" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C21" s="1">
         <v>0</v>
       </c>
       <c r="D21" s="1">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E21" s="1">
-        <f>0.8*$G$3</f>
-        <v>800</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="F21" s="3">
-        <f t="shared" si="0"/>
-        <v>18021800</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+        <f t="shared" ref="F21:F28" si="2">E20+D20*1000+C20*60000+B20*3600000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>400000</v>
       </c>
       <c r="B22" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C22" s="1">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E22" s="1">
-        <f>0.8*$G$3</f>
-        <v>800</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="F22" s="3">
-        <f t="shared" si="0"/>
-        <v>31590800</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
-        <v>510000</v>
+        <v>500000</v>
       </c>
       <c r="B23" s="1">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C23" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E23" s="1">
-        <f>0.87*$G$3</f>
-        <v>870</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="F23" s="3">
-        <f t="shared" si="0"/>
-        <v>61326870</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>600000</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>700000</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>800000</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>900000</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="4">
         <v>1000000</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="B28" s="5">
+        <v>0</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="13"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="13"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
+      <c r="A47" s="10"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" s="13"/>
-      <c r="B49" s="13"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="A49" s="10"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3612,10 +4651,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE2E8F8-3AAF-4919-9E5A-4B56B8585B7D}">
-  <dimension ref="A1:M48"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3630,7 +4669,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -3640,22 +4679,22 @@
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="9" t="s">
         <v>5</v>
       </c>
       <c r="G3">
@@ -3672,27 +4711,27 @@
       </c>
       <c r="M3">
         <f>ROUNDDOWN(J4/86400000,0)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="15">
-        <v>0</v>
-      </c>
-      <c r="B4" s="16">
-        <v>0</v>
-      </c>
-      <c r="C4" s="16">
-        <v>0</v>
-      </c>
-      <c r="D4" s="16">
-        <v>0</v>
-      </c>
-      <c r="E4" s="16">
+      <c r="A4" s="11">
+        <v>0</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12">
         <f>0*$G$3</f>
         <v>0</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="13">
         <f>E4+D4*1000+C4*60000+B4*3600000</f>
         <v>0</v>
       </c>
@@ -3700,475 +4739,756 @@
         <v>11</v>
       </c>
       <c r="J4">
-        <f>0.0003 * J3 * J3 - 16.787 * J3 +657994</f>
-        <v>283870994</v>
+        <f>0.0002 * J3 * J3 - 0.2508 * J3 - 30342</f>
+        <v>199718858</v>
       </c>
       <c r="L4" t="s">
         <v>8</v>
       </c>
       <c r="M4">
         <f>ROUNDDOWN((J4/86400000 - ROUNDDOWN(J4/86400000,0) )* 24,0)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <v>5000</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="3"/>
+        <v>10000</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1">
+        <f>0.45*$G$3</f>
+        <v>450</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" ref="F5:F19" si="0">E5+D5*1000+C5*60000+B5*3600000</f>
+        <v>16450</v>
+      </c>
       <c r="L5" t="s">
         <v>9</v>
       </c>
       <c r="M5">
         <f>ROUNDDOWN(((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60,0)</f>
-        <v>51</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
-        <v>10000</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="3"/>
+        <v>20000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <f>0.97*$G$3</f>
+        <v>970</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>60970</v>
+      </c>
       <c r="L6" t="s">
         <v>10</v>
       </c>
       <c r="M6">
         <f>ROUNDDOWN((((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60 - M5) * 60,0)</f>
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
-        <v>20000</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="3"/>
+        <v>30000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>17</v>
+      </c>
+      <c r="E7" s="1">
+        <f>0.97*$G$3</f>
+        <v>970</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="0"/>
+        <v>137970</v>
+      </c>
       <c r="L7" t="s">
         <v>12</v>
       </c>
       <c r="M7">
         <f>((((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60 - M5) * 60 - M6) * 1000</f>
-        <v>994.00000000599675</v>
+        <v>857.99999998880594</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
-        <v>30000</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="3"/>
+        <v>40000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1">
+        <f>0.6*$G$3</f>
+        <v>600</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="0"/>
+        <v>245600</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
-        <v>40000</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="3"/>
+        <v>50000</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1">
+        <v>41</v>
+      </c>
+      <c r="E9" s="1">
+        <f>0.71*$G$3</f>
+        <v>710</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="0"/>
+        <v>401710</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
-        <v>50000</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="3"/>
+        <v>60000</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1">
+        <v>48</v>
+      </c>
+      <c r="E10" s="1">
+        <f>0.84*$G$3</f>
+        <v>840</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="0"/>
+        <v>588840</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
-        <v>60000</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="3"/>
+        <v>70000</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <f>0.14*$G$3</f>
+        <v>140</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="0"/>
+        <v>842140</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
-        <v>70000</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="3"/>
+        <v>80000</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1">
+        <v>49</v>
+      </c>
+      <c r="E12" s="1">
+        <f>0.1*$G$3</f>
+        <v>100</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="0"/>
+        <v>1129100</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
-        <v>80000</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="3"/>
+        <v>90000</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1">
+        <v>9</v>
+      </c>
+      <c r="E13" s="1">
+        <f>0*$G$3</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="0"/>
+        <v>1509000</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
-        <v>90000</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="3"/>
+        <v>100000</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>31</v>
+      </c>
+      <c r="D14" s="1">
+        <v>53</v>
+      </c>
+      <c r="E14" s="1">
+        <f>0.9*$G$3</f>
+        <v>900</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="0"/>
+        <v>1913900</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
-        <v>100000</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="3"/>
+        <v>120000</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>49</v>
+      </c>
+      <c r="D15" s="1">
+        <v>25</v>
+      </c>
+      <c r="E15" s="1">
+        <f>0.57*$G$3</f>
+        <v>570</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="0"/>
+        <v>2965570</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
-        <v>120000</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="16">
+        <v>140000</v>
+      </c>
+      <c r="B16" s="17">
+        <v>1</v>
+      </c>
+      <c r="C16" s="17">
+        <v>11</v>
+      </c>
+      <c r="D16" s="17">
+        <v>2</v>
+      </c>
+      <c r="E16" s="17">
+        <f>0.53*$G$3</f>
+        <v>530</v>
+      </c>
+      <c r="F16" s="18">
+        <f t="shared" si="0"/>
+        <v>4262530</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
-        <v>140000</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+        <v>160000</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>30</v>
+      </c>
+      <c r="D17" s="1">
+        <v>37</v>
+      </c>
+      <c r="E17" s="1">
+        <f>0.4*$G$3</f>
+        <v>400</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="0"/>
+        <v>5437400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
+        <v>180000</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>51</v>
+      </c>
+      <c r="D18" s="1">
+        <v>58</v>
+      </c>
+      <c r="E18" s="1">
+        <f>0.25*$G$3</f>
+        <v>250</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" si="0"/>
+        <v>6718250</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
         <v>200000</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>14</v>
+      </c>
+      <c r="D19" s="1">
+        <v>59</v>
+      </c>
+      <c r="E19" s="1">
+        <f>0.51*$G$3</f>
+        <v>510</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="0"/>
+        <v>8099510</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
         <v>250000</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" ref="E17:E29" si="1">0*$G$3</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
         <v>300000</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="2">
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" ref="F21:F28" si="2">E20+D20*1000+C20*60000+B20*3600000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
         <v>400000</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
-        <v>510000</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B22" s="1">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
+        <v>500000</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
         <v>600000</v>
       </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="2">
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
         <v>700000</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
         <v>800000</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="2">
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="2">
         <v>900000</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="4">
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="4">
         <v>1000000</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="B28" s="5">
+        <v>0</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0</v>
+      </c>
+      <c r="E28" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" s="13"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="13"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
+      <c r="A47" s="10"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="10"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1345EA7-4FE2-4A5C-83C2-4E073849715A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Optimisation 2 : Lors du traitement d'un nouveau cas, on parcours les chaines existentes pour savoir si la personne contaminatrice de ce cas existe encore. On en profite pour mettre à jour les scores.
</commit_message>
<xml_diff>
--- a/Mesures/1 - Mesures.xlsx
+++ b/Mesures/1 - Mesures.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Documents\Temporaire\FISE2\OPTION1\HPP\Projet_Coronavirus\HPP_Coronavirus_Project\Mesures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2024687-C101-4F66-8BC6-42CD70D2E01C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4873CBEB-FF7A-44B1-884A-A030166E0D0C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" activeTab="2" xr2:uid="{3ECF27EF-CF39-47C0-885E-284BADAE2FC9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" activeTab="3" xr2:uid="{3ECF27EF-CF39-47C0-885E-284BADAE2FC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="3" r:id="rId1"/>
     <sheet name="Optimisation Mono" sheetId="2" r:id="rId2"/>
-    <sheet name="Graphiques" sheetId="5" r:id="rId3"/>
+    <sheet name="Optimisation Mono Parcours" sheetId="6" r:id="rId3"/>
+    <sheet name="Graphiques" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="16">
   <si>
     <t>Itérations</t>
   </si>
@@ -79,12 +80,15 @@
   <si>
     <t>Monothread - Affichage Syso - Correction : chaines unifiées</t>
   </si>
+  <si>
+    <t>Monothread - Affichage Syso - Correction : Parours</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +99,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -313,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -328,13 +338,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1183,6 +1196,428 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.29444772528433943"/>
+                  <c:y val="5.0509259259259261E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Optimisation Mono Parcours'!$A$4:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>400000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Optimisation Mono Parcours'!$F$4:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15680</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59860</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>133760</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>241600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>395540</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>599400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>826730</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1099600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1408140</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1747150</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2528550</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3495410</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29247560</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4ACA-4416-804D-E663619AD459}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="596733903"/>
+        <c:axId val="740232831"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="596733903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="740232831"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="740232831"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="596733903"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1517,6 +1952,158 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Optimisation 2 : Supression d'1 parcours pour l'actualisation des scores lorsqu'on ajoute une nouvelle chain</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Optimisation Mono Parcours'!$A$4:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>400000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Optimisation Mono Parcours'!$F$4:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15680</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59860</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>133760</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>241600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>395540</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>599400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>826730</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1099600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1408140</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1747150</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2528550</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3495410</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29247560</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A282-4840-898F-CD6C4C7B7512}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1532,6 +2119,7 @@
         <c:axId val="737794719"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="200000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1594,6 +2182,8 @@
         <c:axId val="641735583"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="10000000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1661,7 +2251,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1855,6 +2445,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2888,6 +3518,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3489,14 +4635,57 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA0017D9-3F9E-448B-B8DD-F56C7A117C67}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>31750</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>34925</xdr:rowOff>
     </xdr:to>
@@ -3840,14 +5029,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3964,7 +5153,7 @@
       <c r="D6" s="1">
         <v>12</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <f>0.94*$G$3</f>
         <v>940</v>
       </c>
@@ -4287,7 +5476,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" ref="E8:E28" si="1">0*$G$3</f>
+        <f t="shared" ref="E20:E28" si="1">0*$G$3</f>
         <v>0</v>
       </c>
       <c r="F20" s="3">
@@ -4668,14 +5857,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5014,23 +6203,23 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="16">
+      <c r="A16" s="15">
         <v>140000</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="16">
         <v>1</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="16">
         <v>11</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="16">
         <v>2</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="16">
         <f>0.53*$G$3</f>
         <v>530</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="17">
         <f t="shared" si="0"/>
         <v>4262530</v>
       </c>
@@ -5115,7 +6304,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" ref="E17:E29" si="1">0*$G$3</f>
+        <f t="shared" ref="E20:E28" si="1">0*$G$3</f>
         <v>0</v>
       </c>
       <c r="F20" s="3">
@@ -5479,6 +6668,725 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25EF0C5B-BBF3-4CCE-91F4-B28A234D7629}">
+  <dimension ref="A1:M45"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.08984375" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>1000</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>200000</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3">
+        <f>ROUNDDOWN(J4/86400000,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="11">
+        <v>0</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12">
+        <f>0*$G$3</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
+        <f>E4+D4*1000+C4*60000+B4*3600000</f>
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4">
+        <f>0.0002 * J3 * J3 -1.1094 * J3 - 398.25</f>
+        <v>7777721.75</v>
+      </c>
+      <c r="L4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <f>ROUNDDOWN((J4/86400000 - ROUNDDOWN(J4/86400000,0) )* 24,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>10000</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1">
+        <f>0.68*$G$3</f>
+        <v>680</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" ref="F5:F16" si="0">E5+D5*1000+C5*60000+B5*3600000</f>
+        <v>15680</v>
+      </c>
+      <c r="L5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5">
+        <f>ROUNDDOWN(((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60,0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>20000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>59</v>
+      </c>
+      <c r="E6" s="1">
+        <f>0.86*$G$3</f>
+        <v>860</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>59860</v>
+      </c>
+      <c r="L6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6">
+        <f>ROUNDDOWN((((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60 - M5) * 60,0)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>30000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1">
+        <f>0.76*$G$3</f>
+        <v>760</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="0"/>
+        <v>133760</v>
+      </c>
+      <c r="L7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <f>((((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60 - M5) * 60 - M6) * 1000</f>
+        <v>721.74999999990064</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>40000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <f>0.6*$G$3</f>
+        <v>600</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="0"/>
+        <v>241600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>50000</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1">
+        <f>0.54*$G$3</f>
+        <v>540</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="0"/>
+        <v>395540</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>60000</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1">
+        <v>59</v>
+      </c>
+      <c r="E10" s="1">
+        <f>0.4*$G$3</f>
+        <v>400</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="0"/>
+        <v>599400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>70000</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1">
+        <v>46</v>
+      </c>
+      <c r="E11" s="1">
+        <f>0.73*$G$3</f>
+        <v>730</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="0"/>
+        <v>826730</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>80000</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1">
+        <v>19</v>
+      </c>
+      <c r="E12" s="1">
+        <f>0.6*$G$3</f>
+        <v>600</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="0"/>
+        <v>1099600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>90000</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>23</v>
+      </c>
+      <c r="D13" s="1">
+        <v>28</v>
+      </c>
+      <c r="E13" s="1">
+        <f>0.14*$G$3</f>
+        <v>140</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="0"/>
+        <v>1408140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>100000</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>29</v>
+      </c>
+      <c r="D14" s="1">
+        <v>7</v>
+      </c>
+      <c r="E14" s="1">
+        <f>0.15*$G$3</f>
+        <v>150</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="0"/>
+        <v>1747150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>120000</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>42</v>
+      </c>
+      <c r="D15" s="1">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1">
+        <f>0.55*$G$3</f>
+        <v>550</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="0"/>
+        <v>2528550</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" s="19">
+        <v>140000</v>
+      </c>
+      <c r="B16" s="20">
+        <v>0</v>
+      </c>
+      <c r="C16" s="20">
+        <v>58</v>
+      </c>
+      <c r="D16" s="20">
+        <v>15</v>
+      </c>
+      <c r="E16" s="20">
+        <f>0.41*$G$3</f>
+        <v>410</v>
+      </c>
+      <c r="F16" s="21">
+        <f>E16+D16*1000+C16*60000+B16*3600000</f>
+        <v>3495410</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>400000</v>
+      </c>
+      <c r="B17" s="20">
+        <v>8</v>
+      </c>
+      <c r="C17" s="20">
+        <v>7</v>
+      </c>
+      <c r="D17" s="20">
+        <v>27</v>
+      </c>
+      <c r="E17" s="20">
+        <f>0.56*$G$3</f>
+        <v>560</v>
+      </c>
+      <c r="F17" s="21">
+        <f>E17+D17*1000+C17*60000+B17*3600000</f>
+        <v>29247560</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>500000</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" ref="E17:E23" si="1">0*$G$3</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>600000</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" ref="F18:F23" si="2">E18+D18*1000+C18*60000+B18*3600000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>700000</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>800000</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>900000</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="B23" s="5">
+        <v>0</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1345EA7-4FE2-4A5C-83C2-4E073849715A}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Ajout du test représentant l'exemple donné sur le git HPP, ajout d'une fonction dans CoronavirusTopChainCalculator permettant d'actualiser les personnes contaminées et validation des tests faits par Lilian.
</commit_message>
<xml_diff>
--- a/Mesures/1 - Mesures.xlsx
+++ b/Mesures/1 - Mesures.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Documents\Temporaire\FISE2\OPTION1\HPP\Projet_Coronavirus\HPP_Coronavirus_Project\Mesures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4873CBEB-FF7A-44B1-884A-A030166E0D0C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C776BEB-B57E-42AF-AE1E-47CE43EE487B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" activeTab="3" xr2:uid="{3ECF27EF-CF39-47C0-885E-284BADAE2FC9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" firstSheet="2" activeTab="4" xr2:uid="{3ECF27EF-CF39-47C0-885E-284BADAE2FC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="3" r:id="rId1"/>
     <sheet name="Optimisation Mono" sheetId="2" r:id="rId2"/>
     <sheet name="Optimisation Mono Parcours" sheetId="6" r:id="rId3"/>
-    <sheet name="Graphiques" sheetId="5" r:id="rId4"/>
+    <sheet name="Optimisation Mono Accès" sheetId="7" r:id="rId4"/>
+    <sheet name="Graphiques" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="17">
   <si>
     <t>Itérations</t>
   </si>
@@ -82,6 +83,9 @@
   </si>
   <si>
     <t>Monothread - Affichage Syso - Correction : Parours</t>
+  </si>
+  <si>
+    <t>Monothread - Affichage Syso - Correction : Lecture 1 seule donnée à la fois</t>
   </si>
 </sst>
 </file>
@@ -342,12 +346,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1618,6 +1622,549 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.29444772528433943"/>
+                  <c:y val="5.0509259259259261E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Optimisation Mono Accès'!$A$4:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>253000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>305000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>805000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>900000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Optimisation Mono Accès'!$F$4:$F$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8140</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20430</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37490</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>58360</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72880</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>93720</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>119670</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>148810</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>201110</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>248720</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>308110</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>379710</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>592660</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>798730</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1338300</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2084860</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2989570</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4099920</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5377740</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6460450</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7802500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-90B3-4B6F-8D67-8A6CC64D4EFC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="596733903"/>
+        <c:axId val="740232831"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="596733903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="740232831"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="740232831"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="596733903"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Temps des optimisations sur les 100000 premières itérations</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -2104,6 +2651,224 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Optimisation 3 : Supression de la lecture des 3 données des pays à chaque fois, une seule lecture par itération</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Optimisation Mono Accès'!$A$4:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>253000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>305000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>805000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>900000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Optimisation Mono Accès'!$F$4:$F$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8140</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20430</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37490</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>58360</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72880</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>93720</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>119670</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>148810</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>201110</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>248720</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>308110</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>379710</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>592660</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>798730</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1338300</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2084860</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2989570</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4099920</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5377740</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6460450</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7802500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D4D4-4B2C-9BF1-82A103D2A311}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2119,7 +2884,7 @@
         <c:axId val="737794719"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="200000"/>
+          <c:max val="100000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2182,7 +2947,7 @@
         <c:axId val="641735583"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="10000000"/>
+          <c:max val="2500000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2485,6 +3250,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4034,6 +4839,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4678,16 +5999,59 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>31750</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE29A9DF-F212-4298-9AB0-A98D53C705C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>748927</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>279027</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>112058</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5029,14 +6393,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5857,14 +7221,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6686,14 +8050,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6786,7 +8150,7 @@
         <v>680</v>
       </c>
       <c r="F5" s="3">
-        <f t="shared" ref="F5:F16" si="0">E5+D5*1000+C5*60000+B5*3600000</f>
+        <f t="shared" ref="F5:F15" si="0">E5+D5*1000+C5*60000+B5*3600000</f>
         <v>15680</v>
       </c>
       <c r="L5" t="s">
@@ -7032,23 +8396,23 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="19">
+      <c r="A16" s="18">
         <v>140000</v>
       </c>
-      <c r="B16" s="20">
-        <v>0</v>
-      </c>
-      <c r="C16" s="20">
+      <c r="B16" s="19">
+        <v>0</v>
+      </c>
+      <c r="C16" s="19">
         <v>58</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="19">
         <v>15</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="19">
         <f>0.41*$G$3</f>
         <v>410</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="20">
         <f>E16+D16*1000+C16*60000+B16*3600000</f>
         <v>3495410</v>
       </c>
@@ -7057,20 +8421,20 @@
       <c r="A17" s="2">
         <v>400000</v>
       </c>
-      <c r="B17" s="20">
+      <c r="B17" s="19">
         <v>8</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="19">
         <v>7</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="19">
         <v>27</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="19">
         <f>0.56*$G$3</f>
         <v>560</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="20">
         <f>E17+D17*1000+C17*60000+B17*3600000</f>
         <v>29247560</v>
       </c>
@@ -7089,7 +8453,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" ref="E17:E23" si="1">0*$G$3</f>
+        <f t="shared" ref="E18:E23" si="1">0*$G$3</f>
         <v>0</v>
       </c>
       <c r="F18" s="3">
@@ -7114,7 +8478,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="3">
-        <f t="shared" ref="F18:F23" si="2">E18+D18*1000+C18*60000+B18*3600000</f>
+        <f t="shared" ref="F19:F23" si="2">E18+D18*1000+C18*60000+B18*3600000</f>
         <v>0</v>
       </c>
     </row>
@@ -7387,11 +8751,841 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A220A8D-AF89-4CDB-A8E7-536CBD14EEB8}">
+  <dimension ref="A1:M50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.08984375" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+    </row>
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>1000</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>1000000</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3">
+        <f>ROUNDDOWN(J4/86400000,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="11">
+        <v>0</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12">
+        <f>0*$G$3</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
+        <f>E4+D4*1000+C4*60000+B4*3600000</f>
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4">
+        <f>7*10^(-6) * J3 * J3 + 0.644* J3 - 24800</f>
+        <v>7619200</v>
+      </c>
+      <c r="L4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <f>ROUNDDOWN((J4/86400000 - ROUNDDOWN(J4/86400000,0) )* 24,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>10000</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <f>0.62*$G$3</f>
+        <v>620</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" ref="F5:F7" si="0">E5+D5*1000+C5*60000+B5*3600000</f>
+        <v>620</v>
+      </c>
+      <c r="L5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5">
+        <f>ROUNDDOWN(((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>20000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <f>0.15*$G$3</f>
+        <v>150</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>2150</v>
+      </c>
+      <c r="L6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6">
+        <f>ROUNDDOWN((((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60 - M5) * 60,0)</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>30000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1">
+        <f>0.14*$G$3</f>
+        <v>140</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="0"/>
+        <v>8140</v>
+      </c>
+      <c r="L7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <f>((((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60 - M5) * 60 - M6) * 1000</f>
+        <v>199.99999999966178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>40000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1">
+        <f>0.43*$G$3</f>
+        <v>430</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" ref="F8:F16" si="1">E8+D8*1000+C8*60000+B8*3600000</f>
+        <v>20430</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>50000</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>37</v>
+      </c>
+      <c r="E9" s="1">
+        <f>0.49*$G$3</f>
+        <v>490</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="1"/>
+        <v>37490</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>60000</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>51</v>
+      </c>
+      <c r="E10" s="1">
+        <f>0.6*$G$3</f>
+        <v>600</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="1"/>
+        <v>51600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>70000</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>58</v>
+      </c>
+      <c r="E11" s="1">
+        <f>0.36*$G$3</f>
+        <v>360</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="1"/>
+        <v>58360</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>80000</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1">
+        <f>0.88*$G$3</f>
+        <v>880</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="1"/>
+        <v>72880</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>90000</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>33</v>
+      </c>
+      <c r="E13" s="1">
+        <f>0.72*$G$3</f>
+        <v>720</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="1"/>
+        <v>93720</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>100000</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>59</v>
+      </c>
+      <c r="E14" s="1">
+        <f>0.67*$G$3</f>
+        <v>670</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="1"/>
+        <v>119670</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>120000</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>28</v>
+      </c>
+      <c r="E15" s="1">
+        <f>0.81*$G$3</f>
+        <v>810</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="1"/>
+        <v>148810</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" s="18">
+        <v>140000</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>21</v>
+      </c>
+      <c r="E16" s="1">
+        <f>0.11*$G$3</f>
+        <v>110</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="1"/>
+        <v>201110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="18">
+        <v>160000</v>
+      </c>
+      <c r="B17" s="19">
+        <v>0</v>
+      </c>
+      <c r="C17" s="19">
+        <v>4</v>
+      </c>
+      <c r="D17" s="19">
+        <v>8</v>
+      </c>
+      <c r="E17" s="19">
+        <f>0.72*$G$3</f>
+        <v>720</v>
+      </c>
+      <c r="F17" s="20">
+        <f>E17+D17*1000+C17*60000+B17*3600000</f>
+        <v>248720</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="18">
+        <v>180000</v>
+      </c>
+      <c r="B18" s="19">
+        <v>0</v>
+      </c>
+      <c r="C18" s="19">
+        <v>5</v>
+      </c>
+      <c r="D18" s="19">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" ref="E18:E21" si="2">0.11*$G$3</f>
+        <v>110</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" ref="F18:F20" si="3">E18+D18*1000+C18*60000+B18*3600000</f>
+        <v>308110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="18">
+        <v>200000</v>
+      </c>
+      <c r="B19" s="19">
+        <v>0</v>
+      </c>
+      <c r="C19" s="19">
+        <v>6</v>
+      </c>
+      <c r="D19" s="19">
+        <v>19</v>
+      </c>
+      <c r="E19" s="19">
+        <f>0.71*$G$3</f>
+        <v>710</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="3"/>
+        <v>379710</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="18">
+        <v>253000</v>
+      </c>
+      <c r="B20" s="19">
+        <v>0</v>
+      </c>
+      <c r="C20" s="19">
+        <v>9</v>
+      </c>
+      <c r="D20" s="19">
+        <v>52</v>
+      </c>
+      <c r="E20" s="1">
+        <f>0.66*$G$3</f>
+        <v>660</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="3"/>
+        <v>592660</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="18">
+        <v>305000</v>
+      </c>
+      <c r="B21" s="19">
+        <v>0</v>
+      </c>
+      <c r="C21" s="19">
+        <v>13</v>
+      </c>
+      <c r="D21" s="19">
+        <v>18</v>
+      </c>
+      <c r="E21" s="19">
+        <f>0.73*$G$3</f>
+        <v>730</v>
+      </c>
+      <c r="F21" s="20">
+        <f>E21+D21*1000+C21*60000+B21*3600000</f>
+        <v>798730</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>400000</v>
+      </c>
+      <c r="B22" s="19">
+        <v>0</v>
+      </c>
+      <c r="C22" s="19">
+        <v>22</v>
+      </c>
+      <c r="D22" s="19">
+        <v>18</v>
+      </c>
+      <c r="E22" s="19">
+        <f>0.3*$G$3</f>
+        <v>300</v>
+      </c>
+      <c r="F22" s="20">
+        <f>E22+D22*1000+C22*60000+B22*3600000</f>
+        <v>1338300</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>500000</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <v>34</v>
+      </c>
+      <c r="D23" s="1">
+        <v>44</v>
+      </c>
+      <c r="E23" s="1">
+        <f>0.86*$G$3</f>
+        <v>860</v>
+      </c>
+      <c r="F23" s="20">
+        <f>E23+D23*1000+C23*60000+B23*3600000</f>
+        <v>2084860</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
+        <v>600000</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
+        <v>49</v>
+      </c>
+      <c r="D24" s="1">
+        <v>49</v>
+      </c>
+      <c r="E24" s="1">
+        <f>0.57*$G$3</f>
+        <v>570</v>
+      </c>
+      <c r="F24" s="20">
+        <f t="shared" ref="F24:F28" si="4">E24+D24*1000+C24*60000+B24*3600000</f>
+        <v>2989570</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
+        <v>700000</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1">
+        <v>8</v>
+      </c>
+      <c r="D25" s="1">
+        <v>19</v>
+      </c>
+      <c r="E25" s="1">
+        <f>0.92*$G$3</f>
+        <v>920</v>
+      </c>
+      <c r="F25" s="20">
+        <f t="shared" si="4"/>
+        <v>4099920</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
+        <v>805000</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>29</v>
+      </c>
+      <c r="D26" s="1">
+        <v>37</v>
+      </c>
+      <c r="E26" s="1">
+        <f>0.74*$G$3</f>
+        <v>740</v>
+      </c>
+      <c r="F26" s="20">
+        <f t="shared" si="4"/>
+        <v>5377740</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="2">
+        <v>900000</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1">
+        <v>47</v>
+      </c>
+      <c r="D27" s="1">
+        <v>40</v>
+      </c>
+      <c r="E27" s="1">
+        <f>0.45*$G$3</f>
+        <v>450</v>
+      </c>
+      <c r="F27" s="20">
+        <f t="shared" si="4"/>
+        <v>6460450</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="B28" s="5">
+        <v>2</v>
+      </c>
+      <c r="C28" s="5">
+        <v>10</v>
+      </c>
+      <c r="D28" s="5">
+        <v>2</v>
+      </c>
+      <c r="E28" s="5">
+        <f>0.5*$G$3</f>
+        <v>500</v>
+      </c>
+      <c r="F28" s="20">
+        <f t="shared" si="4"/>
+        <v>7802500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="10"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="10"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1345EA7-4FE2-4A5C-83C2-4E073849715A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Ajout des fichiers de résultats et modifications mineures
</commit_message>
<xml_diff>
--- a/Mesures/1 - Mesures.xlsx
+++ b/Mesures/1 - Mesures.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Documents\Temporaire\FISE2\OPTION1\HPP\Projet_Coronavirus\HPP_Coronavirus_Project\Mesures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C776BEB-B57E-42AF-AE1E-47CE43EE487B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B8B12F-CC6C-4323-93BB-B1C8597D31C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" firstSheet="2" activeTab="4" xr2:uid="{3ECF27EF-CF39-47C0-885E-284BADAE2FC9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" firstSheet="3" activeTab="5" xr2:uid="{3ECF27EF-CF39-47C0-885E-284BADAE2FC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="3" r:id="rId1"/>
     <sheet name="Optimisation Mono" sheetId="2" r:id="rId2"/>
     <sheet name="Optimisation Mono Parcours" sheetId="6" r:id="rId3"/>
     <sheet name="Optimisation Mono Accès" sheetId="7" r:id="rId4"/>
-    <sheet name="Graphiques" sheetId="5" r:id="rId5"/>
+    <sheet name="Optimisation MultiThreading" sheetId="8" r:id="rId5"/>
+    <sheet name="Graphiques" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="18">
   <si>
     <t>Itérations</t>
   </si>
@@ -86,6 +87,9 @@
   </si>
   <si>
     <t>Monothread - Affichage Syso - Correction : Lecture 1 seule donnée à la fois</t>
+  </si>
+  <si>
+    <t>Monothread - Affichage Syso - 2 Threads</t>
   </si>
 </sst>
 </file>
@@ -327,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -349,6 +353,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2111,31 +2116,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="fr-FR"/>
-              <a:t>Temps des optimisations sur les 100000 premières itérations</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2174,6 +2154,1123 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.29444772528433943"/>
+                  <c:y val="5.0509259259259261E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Optimisation MultiThreading'!$A$4:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Optimisation MultiThreading'!$F$4:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3880</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6730</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11360</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20850</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37130</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>58330</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>85830</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>120300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>205650</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>302740</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>425730</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>557990</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>709370</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16570810</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9247-4C32-ABD2-86256112EDDC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="596733903"/>
+        <c:axId val="740232831"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="596733903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="740232831"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="740232831"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="596733903"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Temps des optimisations sur les 100000 premières itérations</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Programme fonctionnel initial</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Base!$A$4:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Base!$F$4:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18240</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72940</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>191340</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>341210</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>561320</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>830530</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1118400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1441280</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1821780</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2252660</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3205080</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4326370</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5770790</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7102430</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8451140</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000015-8888-4CB9-A0AC-030471A3FD63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Optimisation 1 - Ajout d'un indice indiquant la première personne dont score &gt; 0</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Optimisation Mono'!$A$4:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Optimisation Mono'!$F$4:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16450</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60970</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>137970</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>245600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>401710</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>588840</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>842140</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1129100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1509000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1913900</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2965570</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4262530</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5437400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6718250</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8099510</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000016-8888-4CB9-A0AC-030471A3FD63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Optimisation 2 : Supression d'1 parcours pour l'actualisation des scores lorsqu'on ajoute une nouvelle chain</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Optimisation Mono Parcours'!$A$4:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>400000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Optimisation Mono Parcours'!$F$4:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15680</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59860</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>133760</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>241600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>395540</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>599400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>826730</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1099600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1408140</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1747150</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2528550</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3495410</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29247560</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000017-8888-4CB9-A0AC-030471A3FD63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Optimisation 3 : Supression de la lecture des 3 données des pays à chaque fois, une seule lecture par itération</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Optimisation Mono Accès'!$A$4:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>253000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>305000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>700000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>805000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>900000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Optimisation Mono Accès'!$F$4:$F$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8140</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20430</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37490</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>58360</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72880</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>93720</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>119670</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>148810</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>201110</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>248720</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>308110</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>379710</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>592660</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>798730</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1338300</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2084860</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2989570</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4099920</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5377740</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6460450</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7802500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000018-8888-4CB9-A0AC-030471A3FD63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Optimisation 4 - MultiThreading</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Optimisation MultiThreading'!$A$4:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Optimisation MultiThreading'!$F$4:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3880</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6730</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11360</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20850</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37130</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>58330</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>85830</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>120300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000019-8888-4CB9-A0AC-030471A3FD63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="5"/>
           <c:tx>
             <c:v>Programme fonctionnel initial</c:v>
           </c:tx>
@@ -2331,13 +3428,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8458-4175-AE98-42E7A1A99229}"/>
+              <c16:uniqueId val="{00000008-8888-4CB9-A0AC-030471A3FD63}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="6"/>
           <c:tx>
             <c:v>Optimisation 1 - Ajout d'un indice indiquant la première personne dont score &gt; 0</c:v>
           </c:tx>
@@ -2495,13 +3592,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-8458-4175-AE98-42E7A1A99229}"/>
+              <c16:uniqueId val="{0000000B-8888-4CB9-A0AC-030471A3FD63}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="7"/>
           <c:tx>
             <c:v>Optimisation 2 : Supression d'1 parcours pour l'actualisation des scores lorsqu'on ajoute une nouvelle chain</c:v>
           </c:tx>
@@ -2647,13 +3744,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-A282-4840-898F-CD6C4C7B7512}"/>
+              <c16:uniqueId val="{0000000E-8888-4CB9-A0AC-030471A3FD63}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="8"/>
           <c:tx>
             <c:v>Optimisation 3 : Supression de la lecture des 3 données des pays à chaque fois, une seule lecture par itération</c:v>
           </c:tx>
@@ -2865,7 +3962,141 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-D4D4-4B2C-9BF1-82A103D2A311}"/>
+              <c16:uniqueId val="{00000011-8888-4CB9-A0AC-030471A3FD63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:v>Optimisation 4 - MultiThreading</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Optimisation MultiThreading'!$A$4:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Optimisation MultiThreading'!$F$4:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3880</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6730</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11360</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20850</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37130</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>58330</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>85830</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>120300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000014-8888-4CB9-A0AC-030471A3FD63}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2949,6 +4180,600 @@
           <c:orientation val="minMax"/>
           <c:max val="2500000"/>
           <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="737794719"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>Temps des optimisations sur les 200000 premières itérations</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Optimisation 3 : Supression de la lecture des 3 données des pays à chaque fois, une seule lecture par itération</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Optimisation Mono Accès'!$A$4:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Optimisation Mono Accès'!$F$4:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8140</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20430</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37490</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>51600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>58360</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72880</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>93720</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>119670</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>148810</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>201110</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>248720</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>308110</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>379710</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-6D62-4D8C-888E-160104B9FD36}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Optimisation 4 - MultiThreading</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Optimisation MultiThreading'!$A$4:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Optimisation MultiThreading'!$F$4:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3880</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6730</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11360</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20850</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37130</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>58330</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>85830</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>120300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>205650</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>302740</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>425730</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>557990</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>709370</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-6D62-4D8C-888E-160104B9FD36}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="737794719"/>
+        <c:axId val="641735583"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="737794719"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="200000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="641735583"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="641735583"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3290,6 +5115,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5355,6 +7220,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6042,6 +8423,49 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1ED04DFE-6E3D-4583-8188-2E4F7A5F2B94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>748927</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -6071,6 +8495,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>716642</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>36286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>246742</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>148344</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42DE79DA-F697-4161-913B-304EDD62D235}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6393,14 +8855,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -7221,14 +9683,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -8050,14 +10512,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -8754,8 +11216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A220A8D-AF89-4CDB-A8E7-536CBD14EEB8}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8769,14 +11231,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -9172,7 +11634,7 @@
         <v>8</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" ref="E18:E21" si="2">0.11*$G$3</f>
+        <f t="shared" ref="E18" si="2">0.11*$G$3</f>
         <v>110</v>
       </c>
       <c r="F18" s="3">
@@ -9581,11 +12043,671 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D302646E-D5B8-428B-9312-A9C4AFBE8DEF}">
+  <dimension ref="A1:M42"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.08984375" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+    </row>
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>1000</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>1000000</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3">
+        <f>ROUNDDOWN(J4/86400000,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="11">
+        <v>0</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12">
+        <f>0*$G$3</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
+        <f>E4+D4*1000+C4*60000+B4*3600000</f>
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4">
+        <f>2*10^(-5) * J3 * J3 + 0.1536* J3 - 29051</f>
+        <v>20124549</v>
+      </c>
+      <c r="L4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <f>ROUNDDOWN((J4/86400000 - ROUNDDOWN(J4/86400000,0) )* 24,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>10000</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <f>0.62*$G$3</f>
+        <v>620</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" ref="F5:F16" si="0">E5+D5*1000+C5*60000+B5*3600000</f>
+        <v>620</v>
+      </c>
+      <c r="L5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5">
+        <f>ROUNDDOWN(((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60,0)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>20000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <f>0.95*$G$3</f>
+        <v>950</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>1950</v>
+      </c>
+      <c r="L6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6">
+        <f>ROUNDDOWN((((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60 - M5) * 60,0)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>30000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <f>0.88*$G$3</f>
+        <v>880</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="0"/>
+        <v>3880</v>
+      </c>
+      <c r="L7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <f>((((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60 - M5) * 60 - M6) * 1000</f>
+        <v>549.00000000108662</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>40000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1">
+        <f>0.73*$G$3</f>
+        <v>730</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="0"/>
+        <v>6730</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>50000</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1">
+        <f>0.36*$G$3</f>
+        <v>360</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="0"/>
+        <v>11360</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>60000</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>20</v>
+      </c>
+      <c r="E10" s="1">
+        <f>0.85*$G$3</f>
+        <v>850</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="0"/>
+        <v>20850</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>70000</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>37</v>
+      </c>
+      <c r="E11" s="1">
+        <f>0.13*$G$3</f>
+        <v>130</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="0"/>
+        <v>37130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>80000</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>58</v>
+      </c>
+      <c r="E12" s="1">
+        <f>0.33*$G$3</f>
+        <v>330</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="0"/>
+        <v>58330</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>90000</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>25</v>
+      </c>
+      <c r="E13" s="1">
+        <f>0.83*$G$3</f>
+        <v>830</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="0"/>
+        <v>85830</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>100000</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <f>0.3*$G$3</f>
+        <v>300</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="0"/>
+        <v>120300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>120000</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>25</v>
+      </c>
+      <c r="E15" s="1">
+        <f>0.65*$G$3</f>
+        <v>650</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="0"/>
+        <v>205650</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" s="18">
+        <v>140000</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1">
+        <f>0.74*$G$3</f>
+        <v>740</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="0"/>
+        <v>302740</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="18">
+        <v>160000</v>
+      </c>
+      <c r="B17" s="19">
+        <v>0</v>
+      </c>
+      <c r="C17" s="19">
+        <v>7</v>
+      </c>
+      <c r="D17" s="19">
+        <v>5</v>
+      </c>
+      <c r="E17" s="19">
+        <f>0.73*$G$3</f>
+        <v>730</v>
+      </c>
+      <c r="F17" s="20">
+        <f>E17+D17*1000+C17*60000+B17*3600000</f>
+        <v>425730</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="18">
+        <v>180000</v>
+      </c>
+      <c r="B18" s="19">
+        <v>0</v>
+      </c>
+      <c r="C18" s="19">
+        <v>9</v>
+      </c>
+      <c r="D18" s="19">
+        <v>17</v>
+      </c>
+      <c r="E18" s="1">
+        <f>0.99*$G$3</f>
+        <v>990</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" ref="F18:F19" si="1">E18+D18*1000+C18*60000+B18*3600000</f>
+        <v>557990</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="18">
+        <v>200000</v>
+      </c>
+      <c r="B19" s="19">
+        <v>0</v>
+      </c>
+      <c r="C19" s="19">
+        <v>11</v>
+      </c>
+      <c r="D19" s="19">
+        <v>49</v>
+      </c>
+      <c r="E19" s="19">
+        <f>0.37*$G$3</f>
+        <v>370</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="1"/>
+        <v>709370</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="B20" s="21">
+        <v>4</v>
+      </c>
+      <c r="C20" s="21">
+        <v>36</v>
+      </c>
+      <c r="D20" s="21">
+        <v>10</v>
+      </c>
+      <c r="E20" s="21">
+        <f>0.81*$G$3</f>
+        <v>810</v>
+      </c>
+      <c r="F20" s="17">
+        <f t="shared" ref="F20" si="2">E20+D20*1000+C20*60000+B20*3600000</f>
+        <v>16570810</v>
+      </c>
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1345EA7-4FE2-4A5C-83C2-4E073849715A}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Ajout du schema de principe présenté, des résultats sur le fichier de 1000000, modifications de l'excel présentant les mesures...
</commit_message>
<xml_diff>
--- a/Mesures/1 - Mesures.xlsx
+++ b/Mesures/1 - Mesures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Documents\Temporaire\FISE2\OPTION1\HPP\Projet_Coronavirus\HPP_Coronavirus_Project\Mesures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B8B12F-CC6C-4323-93BB-B1C8597D31C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AD3401-984C-40E7-8A49-09B198F39637}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" firstSheet="3" activeTab="5" xr2:uid="{3ECF27EF-CF39-47C0-885E-284BADAE2FC9}"/>
   </bookViews>
@@ -449,6 +449,57 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.15497725284339459"/>
+                  <c:y val="2.4380650335374746E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Base!$A$4:$A$19</c:f>
@@ -8841,7 +8892,7 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8926,15 +8977,15 @@
         <v>11</v>
       </c>
       <c r="J4">
-        <f>0.0002 * J3 * J3 - 0.1033 * J3 - 22875</f>
-        <v>199873825</v>
+        <f>0.0002 * J3 * J3 + 3.0616 * J3 - 63270</f>
+        <v>202998330</v>
       </c>
       <c r="L4" t="s">
         <v>8</v>
       </c>
       <c r="M4">
         <f>ROUNDDOWN((J4/86400000 - ROUNDDOWN(J4/86400000,0) )* 24,0)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
@@ -8963,7 +9014,7 @@
       </c>
       <c r="M5">
         <f>ROUNDDOWN(((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60,0)</f>
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -8992,7 +9043,7 @@
       </c>
       <c r="M6">
         <f>ROUNDDOWN((((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60 - M5) * 60,0)</f>
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
@@ -9021,7 +9072,7 @@
       </c>
       <c r="M7">
         <f>((((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60 - M5) * 60 - M6) * 1000</f>
-        <v>824.99999999083684</v>
+        <v>330.00000000566843</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
@@ -10498,7 +10549,7 @@
   <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10548,14 +10599,14 @@
         <v>6</v>
       </c>
       <c r="J3">
-        <v>200000</v>
+        <v>1000000</v>
       </c>
       <c r="L3" t="s">
         <v>7</v>
       </c>
       <c r="M3">
         <f>ROUNDDOWN(J4/86400000,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
@@ -10584,14 +10635,14 @@
       </c>
       <c r="J4">
         <f>0.0002 * J3 * J3 -1.1094 * J3 - 398.25</f>
-        <v>7777721.75</v>
+        <v>198890201.75</v>
       </c>
       <c r="L4" t="s">
         <v>8</v>
       </c>
       <c r="M4">
         <f>ROUNDDOWN((J4/86400000 - ROUNDDOWN(J4/86400000,0) )* 24,0)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
@@ -10620,7 +10671,7 @@
       </c>
       <c r="M5">
         <f>ROUNDDOWN(((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60,0)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -10649,7 +10700,7 @@
       </c>
       <c r="M6">
         <f>ROUNDDOWN((((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60 - M5) * 60,0)</f>
-        <v>37</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
@@ -10678,7 +10729,7 @@
       </c>
       <c r="M7">
         <f>((((J4/86400000-ROUNDDOWN(J4/86400000,0))*24-M4)*60 - M5) * 60 - M6) * 1000</f>
-        <v>721.74999999990064</v>
+        <v>201.75000000705268</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
@@ -11217,7 +11268,7 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:F19"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12047,7 +12098,7 @@
   <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12706,8 +12757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1345EA7-4FE2-4A5C-83C2-4E073849715A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>